<commit_message>
importar personas y activos
</commit_message>
<xml_diff>
--- a/sqat/public/excel/PlantillaActivos.xlsx
+++ b/sqat/public/excel/PlantillaActivos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigoalonsodomingu\Desktop\proyectos\Sistema-Gestor-de-Activos\sqat\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1B01C1-8150-4693-A393-B75F390B4A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7F1489-D751-4C7A-BEBF-5FCB4DCEA81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B072EA93-721B-4733-98FD-913102C38635}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Tipo de activo</t>
   </si>
   <si>
-    <t xml:space="preserve">Precio </t>
+    <t>Ubicación</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
detalles en crear usuario
</commit_message>
<xml_diff>
--- a/sqat/public/excel/PlantillaActivos.xlsx
+++ b/sqat/public/excel/PlantillaActivos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigoalonsodomingu\Desktop\proyectos\Sistema-Gestor-de-Activos\sqat\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7F1489-D751-4C7A-BEBF-5FCB4DCEA81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662DE122-5C84-45E9-B7AA-24326B8D5EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B072EA93-721B-4733-98FD-913102C38635}"/>
   </bookViews>
@@ -35,6 +35,54 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>rodrigo alonso dominguez araya</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E71583BB-82EE-44D0-A546-0C28D8E2D591}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CHILLAN
+COSMITO
+LINARES
+LOS ANGELES
+MOLINA
+OSORNO
+PAINE
+PARRAL
+QUEPE
+QUILICURA
+RAPACO
+ROSARIO NORTE
+SAN FERNANDO
+CONCEPCION
+NOVICIADO</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
@@ -57,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,16 +113,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,12 +156,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,36 +513,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FE0A42-BCEF-4CBB-B7DE-D851AD860034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FE0A42-BCEF-4CBB-B7DE-D851AD860034}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>